<commit_message>
semichaos door opschonen in loops
</commit_message>
<xml_diff>
--- a/Running Dinner eerste oplossing 2023 v2.xlsx
+++ b/Running Dinner eerste oplossing 2023 v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School Software\Vscode Omgeving\or5\RunningDinnerV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CC868D-2880-410B-9D60-CB7A989A99D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA60D8CF-AF7C-423C-849C-AD13F8728616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -647,7 +647,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1000,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,7 +1237,7 @@
         <v>163</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
2optwerkt, milou dr code staat er nu nog in
</commit_message>
<xml_diff>
--- a/Running Dinner eerste oplossing 2023 v2.xlsx
+++ b/Running Dinner eerste oplossing 2023 v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School Software\Vscode Omgeving\or5\RunningDinnerV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA60D8CF-AF7C-423C-849C-AD13F8728616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CCA610-3E4D-4629-AD64-19F7914A9D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,7 +629,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,19 +645,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -692,7 +692,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -999,13 +999,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="7.109375" bestFit="1" customWidth="1"/>
@@ -1038,157 +1037,181 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
-      </c>
-      <c r="F2" t="s">
-        <v>147</v>
+        <v>106</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
         <v>115</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F3" t="s">
-        <v>126</v>
+        <v>106</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>120</v>
+        <v>102</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>103</v>
-      </c>
-      <c r="C5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E5" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" t="s">
-        <v>137</v>
+      <c r="H5">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F6" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
       </c>
       <c r="H6">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="F7" t="s">
-        <v>187</v>
+        <v>134</v>
       </c>
       <c r="G7" t="s">
         <v>3</v>
       </c>
       <c r="H7">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="D8" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="E8" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="F8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H8">
         <v>6</v>
@@ -1196,25 +1219,25 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="F9" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H9">
         <v>6</v>
@@ -1222,129 +1245,129 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E10" t="s">
         <v>163</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>104</v>
+      <c r="F10" t="s">
+        <v>129</v>
       </c>
       <c r="G10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="G11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="G12" t="s">
         <v>3</v>
       </c>
       <c r="H12">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E13" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="F13" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="G13" t="s">
         <v>3</v>
       </c>
       <c r="H13">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s">
-        <v>123</v>
+        <v>94</v>
       </c>
       <c r="E14" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="F14" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="G14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H14">
         <v>6</v>
@@ -1352,25 +1375,25 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>169</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E15" t="s">
         <v>142</v>
       </c>
       <c r="F15" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="G15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -1378,181 +1401,181 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="C16" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="E16" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
       <c r="F16" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H16">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="E17" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="F17" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="G17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H17">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>131</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="E18" t="s">
         <v>133</v>
       </c>
       <c r="F18" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G18" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="F19" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="G19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="D20" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="E20" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="F20" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="G20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H20">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>138</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="F21" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="G21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H21">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="E22" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="F22" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="G22" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22">
         <v>6</v>
@@ -1560,25 +1583,25 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="E23" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="F23" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="G23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23">
         <v>6</v>
@@ -1586,25 +1609,25 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>157</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="F24" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H24">
         <v>8</v>
@@ -1612,25 +1635,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>16</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>188</v>
       </c>
       <c r="D25" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E25" t="s">
-        <v>155</v>
+        <v>188</v>
       </c>
       <c r="F25" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="G25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H25">
         <v>8</v>
@@ -1638,129 +1661,129 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="D26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>188</v>
       </c>
       <c r="F26" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="G26" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H26">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E27" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H27">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>149</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>189</v>
       </c>
       <c r="D28" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="E28" t="s">
-        <v>113</v>
+        <v>189</v>
       </c>
       <c r="F28" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="G28" t="s">
         <v>3</v>
       </c>
       <c r="H28">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>189</v>
       </c>
       <c r="D29" t="s">
-        <v>148</v>
+        <v>112</v>
       </c>
       <c r="E29" t="s">
-        <v>113</v>
+        <v>189</v>
       </c>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="G29" t="s">
         <v>3</v>
       </c>
       <c r="H29">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>153</v>
+        <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="E30" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="F30" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="G30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H30">
         <v>6</v>
@@ -1768,25 +1791,25 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>95</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="E31" t="s">
-        <v>188</v>
+        <v>95</v>
       </c>
       <c r="F31" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="G31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H31">
         <v>6</v>
@@ -1794,22 +1817,22 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>28</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="F32" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G32" t="s">
         <v>3</v>
@@ -1820,22 +1843,22 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
-        <v>116</v>
+        <v>195</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>100</v>
       </c>
       <c r="F33" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="G33" t="s">
         <v>3</v>
@@ -1846,328 +1869,328 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>30</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>139</v>
+        <v>184</v>
       </c>
       <c r="D34" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
       <c r="F34" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="G34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H34">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>184</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="E35" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="F35" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="G35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H35">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D36" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="E36" t="s">
-        <v>176</v>
+        <v>107</v>
       </c>
       <c r="F36" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G36" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H36">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E37" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="F37" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
       <c r="G37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H37">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D38" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="E38" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="F38" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G38" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H38">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>33</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="D39" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
       <c r="E39" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="F39" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H39">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>42</v>
+        <v>6</v>
       </c>
       <c r="B40" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D40" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="F40" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="G40" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H40">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="E41" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F41" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="G41" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H41">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B42" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="E42" t="s">
         <v>163</v>
       </c>
       <c r="F42" t="s">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="G42" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H42">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s">
         <v>146</v>
       </c>
       <c r="E43" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="F43" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G43" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H43">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="E44" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F44" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="G44" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H44">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E45" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F45" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="G45" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H45">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B46" t="s">
-        <v>173</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="D46" t="s">
-        <v>174</v>
+        <v>94</v>
       </c>
       <c r="E46" t="s">
         <v>189</v>
@@ -2176,33 +2199,33 @@
         <v>108</v>
       </c>
       <c r="G46" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H46">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="E47" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="F47" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="G47" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H47">
         <v>6</v>
@@ -2210,25 +2233,25 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="C48" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D48" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="E48" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="F48" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="G48" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H48">
         <v>6</v>
@@ -2236,137 +2259,149 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>22</v>
+        <v>154</v>
       </c>
       <c r="C49" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="D49" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="E49" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F49" t="s">
         <v>150</v>
       </c>
+      <c r="G49" t="s">
+        <v>4</v>
+      </c>
+      <c r="H49">
+        <v>6</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="D50" t="s">
-        <v>123</v>
+        <v>195</v>
       </c>
       <c r="E50" t="s">
-        <v>184</v>
+        <v>133</v>
       </c>
       <c r="F50" t="s">
-        <v>93</v>
+        <v>139</v>
+      </c>
+      <c r="G50" t="s">
+        <v>4</v>
+      </c>
+      <c r="H50">
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>38</v>
       </c>
       <c r="C51" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="D51" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E51" t="s">
         <v>176</v>
       </c>
       <c r="F51" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="G51" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H51">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="D52" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="E52" t="s">
-        <v>176</v>
+        <v>106</v>
       </c>
       <c r="F52" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="G52" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H52">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
       <c r="C53" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="D53" t="s">
         <v>148</v>
       </c>
       <c r="E53" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="F53" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G53" t="s">
         <v>4</v>
       </c>
       <c r="H53">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="C54" t="s">
         <v>105</v>
       </c>
       <c r="D54" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E54" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="F54" t="s">
         <v>105</v>
@@ -2380,77 +2415,77 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="D55" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="E55" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="F55" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="G55" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H55">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D56" t="s">
         <v>156</v>
       </c>
       <c r="E56" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F56" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="G56" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H56">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>180</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D57" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="E57" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="F57" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="G57" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H57">
         <v>6</v>
@@ -2458,25 +2493,25 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="C58" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="E58" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F58" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
       <c r="G58" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H58">
         <v>6</v>
@@ -2484,45 +2519,45 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>181</v>
+        <v>44</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="D59" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="E59" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="F59" t="s">
-        <v>102</v>
+        <v>143</v>
       </c>
       <c r="G59" t="s">
         <v>4</v>
       </c>
       <c r="H59">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>181</v>
       </c>
       <c r="C60" t="s">
         <v>102</v>
       </c>
       <c r="D60" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
       <c r="E60" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="F60" t="s">
         <v>102</v>
@@ -2536,48 +2571,48 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>21</v>
       </c>
       <c r="C61" t="s">
-        <v>172</v>
+        <v>102</v>
       </c>
       <c r="D61" t="s">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="E61" t="s">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="F61" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="G61" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H61">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C62" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="D62" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="E62" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="F62" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="G62" t="s">
         <v>4</v>
@@ -2588,22 +2623,22 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C63" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="D63" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="E63" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="F63" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="G63" t="s">
         <v>4</v>
@@ -2614,181 +2649,181 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C64" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="D64" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="E64" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="F64" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="G64" t="s">
         <v>4</v>
       </c>
       <c r="H64">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="B65" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C65" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="D65" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="E65" t="s">
-        <v>113</v>
+        <v>167</v>
       </c>
       <c r="F65" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="G65" t="s">
         <v>4</v>
       </c>
       <c r="H65">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
-        <v>182</v>
+        <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="E66" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="F66" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="G66" t="s">
         <v>4</v>
       </c>
       <c r="H66">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="B67" t="s">
-        <v>183</v>
+        <v>17</v>
       </c>
       <c r="C67" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="D67" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="E67" t="s">
         <v>106</v>
       </c>
       <c r="F67" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="G67" t="s">
         <v>4</v>
       </c>
       <c r="H67">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="B68" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C68" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D68" t="s">
         <v>115</v>
       </c>
       <c r="E68" t="s">
-        <v>188</v>
+        <v>107</v>
       </c>
       <c r="F68" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="G68" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H68">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="C69" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D69" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="E69" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="F69" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G69" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H69">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <v>68</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="D70" t="s">
-        <v>171</v>
+        <v>112</v>
       </c>
       <c r="E70" t="s">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="F70" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="G70" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H70">
         <v>6</v>
@@ -2796,25 +2831,25 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <v>69</v>
+        <v>101</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>171</v>
+        <v>147</v>
       </c>
       <c r="D71" t="s">
-        <v>171</v>
+        <v>112</v>
       </c>
       <c r="E71" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="F71" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="G71" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H71">
         <v>6</v>
@@ -2822,77 +2857,77 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <v>70</v>
+        <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
       <c r="C72" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="D72" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="E72" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="F72" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="G72" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H72">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="B73" t="s">
-        <v>62</v>
+        <v>197</v>
       </c>
       <c r="C73" t="s">
-        <v>167</v>
+        <v>93</v>
       </c>
       <c r="D73" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="E73" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F73" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
       <c r="G73" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H73">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="B74" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="C74" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="D74" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E74" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="F74" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="G74" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H74">
         <v>6</v>
@@ -2900,25 +2935,25 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="B75" t="s">
-        <v>186</v>
+        <v>54</v>
       </c>
       <c r="C75" t="s">
-        <v>124</v>
+        <v>187</v>
       </c>
       <c r="D75" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="E75" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F75" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="G75" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H75">
         <v>6</v>
@@ -2926,166 +2961,178 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="B76" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="C76" t="s">
-        <v>114</v>
+        <v>187</v>
       </c>
       <c r="D76" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="E76" t="s">
-        <v>95</v>
+        <v>167</v>
       </c>
       <c r="F76" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
       <c r="G76" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H76">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="B77" t="s">
-        <v>69</v>
+        <v>199</v>
       </c>
       <c r="C77" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D77" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="E77" t="s">
-        <v>159</v>
+        <v>100</v>
       </c>
       <c r="F77" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G77" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H77">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <v>76</v>
+        <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C78" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="D78" t="s">
-        <v>174</v>
+        <v>123</v>
       </c>
       <c r="E78" t="s">
-        <v>188</v>
+        <v>133</v>
       </c>
       <c r="F78" t="s">
-        <v>120</v>
+        <v>147</v>
       </c>
       <c r="G78" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H78">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <v>77</v>
+        <v>13</v>
       </c>
       <c r="B79" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C79" t="s">
-        <v>188</v>
+        <v>123</v>
       </c>
       <c r="D79" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="E79" t="s">
-        <v>188</v>
+        <v>142</v>
       </c>
       <c r="F79" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="G79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H79">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="B80" t="s">
-        <v>48</v>
+        <v>131</v>
       </c>
       <c r="C80" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="D80" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="E80" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="F80" t="s">
-        <v>108</v>
+        <v>139</v>
+      </c>
+      <c r="G80" t="s">
+        <v>2</v>
+      </c>
+      <c r="H80">
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>53</v>
+        <v>135</v>
       </c>
       <c r="C81" t="s">
-        <v>190</v>
+        <v>132</v>
       </c>
       <c r="D81" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="E81" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="F81" t="s">
-        <v>187</v>
+        <v>104</v>
+      </c>
+      <c r="G81" t="s">
+        <v>2</v>
+      </c>
+      <c r="H81">
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="B82" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="C82" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D82" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="E82" t="s">
-        <v>188</v>
+        <v>159</v>
       </c>
       <c r="F82" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="G82" t="s">
         <v>2</v>
@@ -3096,22 +3143,22 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>144</v>
       </c>
       <c r="C83" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D83" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="E83" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="F83" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="G83" t="s">
         <v>2</v>
@@ -3122,126 +3169,126 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="B84" t="s">
-        <v>191</v>
+        <v>47</v>
       </c>
       <c r="C84" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="D84" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="E84" t="s">
-        <v>189</v>
+        <v>106</v>
       </c>
       <c r="F84" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G84" t="s">
         <v>2</v>
       </c>
       <c r="H84">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="B85" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C85" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="D85" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="E85" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F85" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="G85" t="s">
         <v>2</v>
       </c>
       <c r="H85">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B86" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C86" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D86" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
       <c r="E86" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="F86" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="G86" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H86">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="B87" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C87" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D87" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
       <c r="E87" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="F87" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="G87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H87">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="B88" t="s">
-        <v>192</v>
+        <v>59</v>
       </c>
       <c r="C88" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D88" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E88" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="F88" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="G88" t="s">
         <v>2</v>
@@ -3252,22 +3299,22 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="B89" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="C89" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D89" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E89" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="F89" t="s">
-        <v>104</v>
+        <v>147</v>
       </c>
       <c r="G89" t="s">
         <v>2</v>
@@ -3278,103 +3325,103 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="B90" t="s">
-        <v>50</v>
+        <v>164</v>
       </c>
       <c r="C90" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D90" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="E90" t="s">
-        <v>167</v>
+        <v>109</v>
       </c>
       <c r="F90" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="G90" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H90">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="B91" t="s">
-        <v>31</v>
+        <v>165</v>
       </c>
       <c r="C91" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D91" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="E91" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="F91" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="G91" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H91">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="B92" t="s">
-        <v>71</v>
+        <v>173</v>
       </c>
       <c r="C92" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="D92" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="E92" t="s">
         <v>189</v>
       </c>
       <c r="F92" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="G92" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H92">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="B93" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C93" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="D93" t="s">
-        <v>112</v>
+        <v>145</v>
       </c>
       <c r="E93" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
       <c r="F93" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="G93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H93">
         <v>6</v>
@@ -3382,126 +3429,126 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="B94" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C94" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D94" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="E94" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F94" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="G94" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H94">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="B95" t="s">
-        <v>17</v>
+        <v>178</v>
       </c>
       <c r="C95" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="D95" t="s">
-        <v>125</v>
+        <v>172</v>
       </c>
       <c r="E95" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="F95" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G95" t="s">
+        <v>2</v>
+      </c>
+      <c r="H95">
         <v>4</v>
-      </c>
-      <c r="H95">
-        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="B96" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C96" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D96" t="s">
         <v>115</v>
       </c>
       <c r="E96" t="s">
-        <v>107</v>
+        <v>188</v>
       </c>
       <c r="F96" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="G96" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H96">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="B97" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C97" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D97" t="s">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="E97" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="F97" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G97" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H97">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="B98" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C98" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="D98" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="E98" t="s">
-        <v>133</v>
+        <v>176</v>
       </c>
       <c r="F98" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="G98" t="s">
         <v>2</v>
@@ -3512,22 +3559,22 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="B99" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
       <c r="C99" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="D99" t="s">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="E99" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="F99" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="G99" t="s">
         <v>2</v>
@@ -3538,77 +3585,77 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B100" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C100" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="D100" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="E100" t="s">
         <v>95</v>
       </c>
       <c r="F100" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G100" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H100">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="B101" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="C101" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="D101" t="s">
         <v>114</v>
       </c>
       <c r="E101" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="F101" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G101" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H101">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B102" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="C102" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="D102" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="E102" t="s">
-        <v>124</v>
+        <v>188</v>
       </c>
       <c r="F102" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="G102" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H102">
         <v>6</v>
@@ -3616,25 +3663,25 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B103" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="C103" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="D103" t="s">
-        <v>112</v>
+        <v>160</v>
       </c>
       <c r="E103" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="F103" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="G103" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H103">
         <v>6</v>
@@ -3642,117 +3689,129 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B104" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C104" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D104" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="E104" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F104" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G104" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H104">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C105" t="s">
-        <v>194</v>
+        <v>112</v>
       </c>
       <c r="D105" t="s">
-        <v>195</v>
+        <v>112</v>
       </c>
       <c r="E105" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="F105" t="s">
-        <v>110</v>
+        <v>102</v>
+      </c>
+      <c r="G105" t="s">
+        <v>2</v>
+      </c>
+      <c r="H105">
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="B106" t="s">
-        <v>34</v>
+        <v>192</v>
       </c>
       <c r="C106" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="D106" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="E106" t="s">
-        <v>97</v>
+        <v>188</v>
       </c>
       <c r="F106" t="s">
-        <v>110</v>
+        <v>150</v>
+      </c>
+      <c r="G106" t="s">
+        <v>2</v>
+      </c>
+      <c r="H106">
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="B107" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C107" t="s">
-        <v>100</v>
+        <v>156</v>
       </c>
       <c r="D107" t="s">
         <v>156</v>
       </c>
       <c r="E107" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="F107" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="G107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H107">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="C108" t="s">
-        <v>100</v>
+        <v>152</v>
       </c>
       <c r="D108" t="s">
-        <v>195</v>
+        <v>152</v>
       </c>
       <c r="E108" t="s">
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="F108" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G108" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H108">
         <v>6</v>
@@ -3760,50 +3819,62 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B109" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="C109" t="s">
-        <v>196</v>
+        <v>152</v>
       </c>
       <c r="D109" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E109" t="s">
-        <v>184</v>
+        <v>117</v>
       </c>
       <c r="F109" t="s">
-        <v>143</v>
+        <v>128</v>
+      </c>
+      <c r="G109" t="s">
+        <v>2</v>
+      </c>
+      <c r="H109">
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>196</v>
+        <v>101</v>
       </c>
       <c r="D110" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="E110" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="F110" t="s">
-        <v>134</v>
+        <v>139</v>
+      </c>
+      <c r="G110" t="s">
+        <v>2</v>
+      </c>
+      <c r="H110">
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="C111" t="s">
         <v>101</v>
@@ -3812,10 +3883,10 @@
         <v>101</v>
       </c>
       <c r="E111" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="F111" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="G111" t="s">
         <v>2</v>
@@ -3826,22 +3897,22 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
+        <v>119</v>
+      </c>
+      <c r="B112" t="s">
+        <v>23</v>
+      </c>
+      <c r="C112" t="s">
+        <v>195</v>
+      </c>
+      <c r="D112" t="s">
+        <v>195</v>
+      </c>
+      <c r="E112" t="s">
+        <v>97</v>
+      </c>
+      <c r="F112" t="s">
         <v>110</v>
-      </c>
-      <c r="B112" t="s">
-        <v>52</v>
-      </c>
-      <c r="C112" t="s">
-        <v>101</v>
-      </c>
-      <c r="D112" t="s">
-        <v>101</v>
-      </c>
-      <c r="E112" t="s">
-        <v>167</v>
-      </c>
-      <c r="F112" t="s">
-        <v>143</v>
       </c>
       <c r="G112" t="s">
         <v>2</v>
@@ -3852,10 +3923,10 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B113" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C113" t="s">
         <v>195</v>
@@ -3878,366 +3949,294 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B114" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="C114" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
       <c r="D114" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
       <c r="E114" t="s">
-        <v>97</v>
+        <v>155</v>
       </c>
       <c r="F114" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G114" t="s">
         <v>2</v>
       </c>
       <c r="H114">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B115" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C115" t="s">
-        <v>184</v>
+        <v>116</v>
       </c>
       <c r="D115" t="s">
-        <v>171</v>
+        <v>116</v>
       </c>
       <c r="E115" t="s">
-        <v>184</v>
+        <v>109</v>
       </c>
       <c r="F115" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="G115" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H115">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
+        <v>0</v>
+      </c>
+      <c r="B116" t="s">
+        <v>91</v>
+      </c>
+      <c r="C116" t="s">
+        <v>92</v>
+      </c>
+      <c r="D116" t="s">
         <v>112</v>
       </c>
-      <c r="B116" t="s">
-        <v>89</v>
-      </c>
-      <c r="C116" t="s">
-        <v>184</v>
-      </c>
-      <c r="D116" t="s">
-        <v>171</v>
-      </c>
       <c r="E116" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="F116" t="s">
-        <v>150</v>
-      </c>
-      <c r="G116" t="s">
-        <v>3</v>
-      </c>
-      <c r="H116">
-        <v>6</v>
+        <v>147</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
-        <v>113</v>
+        <v>1</v>
       </c>
       <c r="B117" t="s">
-        <v>197</v>
+        <v>96</v>
       </c>
       <c r="C117" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D117" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="E117" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
       <c r="F117" t="s">
-        <v>93</v>
-      </c>
-      <c r="G117" t="s">
-        <v>4</v>
-      </c>
-      <c r="H117">
-        <v>6</v>
+        <v>126</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
-        <v>114</v>
+        <v>2</v>
       </c>
       <c r="B118" t="s">
-        <v>198</v>
+        <v>98</v>
       </c>
       <c r="C118" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D118" t="s">
         <v>94</v>
       </c>
       <c r="E118" t="s">
-        <v>159</v>
+        <v>188</v>
       </c>
       <c r="F118" t="s">
-        <v>93</v>
-      </c>
-      <c r="G118" t="s">
-        <v>4</v>
-      </c>
-      <c r="H118">
-        <v>6</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="B119" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="C119" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D119" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E119" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
       <c r="F119" t="s">
-        <v>105</v>
-      </c>
-      <c r="G119" t="s">
-        <v>3</v>
-      </c>
-      <c r="H119">
-        <v>6</v>
+        <v>137</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
-        <v>116</v>
+        <v>46</v>
       </c>
       <c r="B120" t="s">
-        <v>68</v>
+        <v>22</v>
       </c>
       <c r="C120" t="s">
-        <v>107</v>
+        <v>170</v>
       </c>
       <c r="D120" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="E120" t="s">
-        <v>107</v>
+        <v>184</v>
       </c>
       <c r="F120" t="s">
-        <v>187</v>
-      </c>
-      <c r="G120" t="s">
-        <v>3</v>
-      </c>
-      <c r="H120">
-        <v>6</v>
+        <v>150</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
-        <v>117</v>
+        <v>47</v>
       </c>
       <c r="B121" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="C121" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="D121" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="E121" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="F121" t="s">
-        <v>128</v>
-      </c>
-      <c r="G121" t="s">
-        <v>3</v>
-      </c>
-      <c r="H121">
-        <v>6</v>
+        <v>93</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B122" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C122" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="D122" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="E122" t="s">
-        <v>159</v>
+        <v>95</v>
       </c>
       <c r="F122" t="s">
-        <v>139</v>
-      </c>
-      <c r="G122" t="s">
-        <v>3</v>
-      </c>
-      <c r="H122">
-        <v>6</v>
+        <v>108</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="B123" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C123" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D123" t="s">
-        <v>101</v>
+        <v>156</v>
       </c>
       <c r="E123" t="s">
-        <v>117</v>
+        <v>163</v>
       </c>
       <c r="F123" t="s">
         <v>187</v>
       </c>
-      <c r="G123" t="s">
-        <v>4</v>
-      </c>
-      <c r="H123">
-        <v>6</v>
-      </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B124" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C124" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D124" t="s">
-        <v>132</v>
+        <v>195</v>
       </c>
       <c r="E124" t="s">
-        <v>167</v>
+        <v>97</v>
       </c>
       <c r="F124" t="s">
-        <v>187</v>
-      </c>
-      <c r="G124" t="s">
-        <v>4</v>
-      </c>
-      <c r="H124">
-        <v>6</v>
+        <v>110</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="B125" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="C125" t="s">
-        <v>116</v>
+        <v>194</v>
       </c>
       <c r="D125" t="s">
-        <v>116</v>
+        <v>195</v>
       </c>
       <c r="E125" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="F125" t="s">
-        <v>108</v>
-      </c>
-      <c r="G125" t="s">
-        <v>2</v>
-      </c>
-      <c r="H125">
-        <v>7</v>
+        <v>110</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B126" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C126" t="s">
-        <v>116</v>
+        <v>196</v>
       </c>
       <c r="D126" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="E126" t="s">
-        <v>109</v>
+        <v>184</v>
       </c>
       <c r="F126" t="s">
-        <v>187</v>
-      </c>
-      <c r="G126" t="s">
-        <v>2</v>
-      </c>
-      <c r="H126">
-        <v>7</v>
+        <v>143</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B127" t="s">
-        <v>199</v>
+        <v>81</v>
       </c>
       <c r="C127" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="D127" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E127" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="F127" t="s">
-        <v>122</v>
-      </c>
-      <c r="G127" t="s">
-        <v>4</v>
-      </c>
-      <c r="H127">
-        <v>5</v>
+        <v>134</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
@@ -4282,9 +4281,8 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H129">
-    <sortCondition ref="B1:B129"/>
+    <sortCondition ref="G1:G129"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>